<commit_message>
feat: command line arguments, add: requirements.txt
</commit_message>
<xml_diff>
--- a/temp1.xlsx
+++ b/temp1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramez\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramez\Desktop\New folder (4)\ASU-schedule-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A2532-11D1-4809-A192-061FCE8F8710}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB26FDEC-CE5F-4378-9B7C-FAA44CB1DBA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,25 +441,25 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,35 +750,35 @@
   <cols>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
+    <col min="4" max="4" width="58.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="27"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="2:6" ht="19.149999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="19.7" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="21" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>